<commit_message>
Huge updates: Adding the folder client-only which contains a version of the app where user can upload a pdf file of the ordered product, and the app scans the file, extract the products id and their quantitis and returns how the products should be palletized.
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samis-mac/My Drive/Courses/Fullstack-Development/Palletize/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samis-mac/My Drive/Courses/Fullstack-Development/Palletize-JS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1B03E28-D61C-2C41-AB5E-C80C09D72702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC2A065-AEC1-3340-8BE3-33D575CD79D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32240" yWindow="2540" windowWidth="28040" windowHeight="17440" xr2:uid="{45393510-64A5-C247-9837-CB0B304B2551}"/>
+    <workbookView xWindow="2920" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{45393510-64A5-C247-9837-CB0B304B2551}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,11 +83,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,149 +420,245 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2CFBF6E-060D-1D41-B3E2-9F114B5B9C9B}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="32" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="32" x14ac:dyDescent="0.4">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
+        <v>1112</v>
+      </c>
+      <c r="B2" s="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="32" x14ac:dyDescent="0.4">
+      <c r="A3" s="1">
+        <v>2701</v>
+      </c>
+      <c r="B3" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="32" x14ac:dyDescent="0.4">
+      <c r="A4" s="1">
+        <v>1289</v>
+      </c>
+      <c r="B4" s="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="32" x14ac:dyDescent="0.4">
+      <c r="A5" s="1">
+        <v>1260</v>
+      </c>
+      <c r="B5" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="32" x14ac:dyDescent="0.4">
+      <c r="A6" s="1">
+        <v>1286</v>
+      </c>
+      <c r="B6" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="32" x14ac:dyDescent="0.4">
+      <c r="A7" s="1">
+        <v>2703</v>
+      </c>
+      <c r="B7" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="32" x14ac:dyDescent="0.4">
+      <c r="A8" s="1">
+        <v>327994</v>
+      </c>
+      <c r="B8" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="32" x14ac:dyDescent="0.4">
+      <c r="A9" s="1">
+        <v>2706</v>
+      </c>
+      <c r="B9" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="32" x14ac:dyDescent="0.4">
+      <c r="A10" s="1">
+        <v>1292</v>
+      </c>
+      <c r="B10" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="32" x14ac:dyDescent="0.4">
+      <c r="A11" s="1">
+        <v>7734</v>
+      </c>
+      <c r="B11" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="32" x14ac:dyDescent="0.4">
+      <c r="A12" s="1">
+        <v>63326</v>
+      </c>
+      <c r="B12" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="32" x14ac:dyDescent="0.4">
+      <c r="A13" s="1">
+        <v>7123</v>
+      </c>
+      <c r="B13" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="32" x14ac:dyDescent="0.4">
+      <c r="A14" s="1">
+        <v>1391</v>
+      </c>
+      <c r="B14" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="32" x14ac:dyDescent="0.4">
+      <c r="A15" s="1">
+        <v>9839</v>
+      </c>
+      <c r="B15" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="32" x14ac:dyDescent="0.4">
+      <c r="A16" s="1">
+        <v>5209</v>
+      </c>
+      <c r="B16" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="32" x14ac:dyDescent="0.4">
+      <c r="A17" s="1">
+        <v>1111</v>
+      </c>
+      <c r="B17" s="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="32" x14ac:dyDescent="0.4">
+      <c r="A18" s="1">
+        <v>1161</v>
+      </c>
+      <c r="B18" s="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="32" x14ac:dyDescent="0.4">
+      <c r="A19" s="1">
+        <v>1251</v>
+      </c>
+      <c r="B19" s="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="32" x14ac:dyDescent="0.4">
+      <c r="A20" s="1">
         <v>1311</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B20" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="32" x14ac:dyDescent="0.4">
+      <c r="A21" s="1">
+        <v>1057</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="32" x14ac:dyDescent="0.4">
+      <c r="A22" s="1">
+        <v>3467</v>
+      </c>
+      <c r="B22" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="32" x14ac:dyDescent="0.4">
+      <c r="A23" s="1">
+        <v>1176</v>
+      </c>
+      <c r="B23" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="32" x14ac:dyDescent="0.4">
+      <c r="A24" s="1">
+        <v>5585</v>
+      </c>
+      <c r="B24" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="32" x14ac:dyDescent="0.4">
+      <c r="A25" s="1">
+        <v>1016</v>
+      </c>
+      <c r="B25" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="32" x14ac:dyDescent="0.4">
+      <c r="A26" s="1">
+        <v>1167</v>
+      </c>
+      <c r="B26" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="32" x14ac:dyDescent="0.4">
-      <c r="A3" s="2">
-        <v>10422</v>
-      </c>
-      <c r="B3" s="2">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="32" x14ac:dyDescent="0.4">
-      <c r="A4" s="2">
-        <v>3948</v>
-      </c>
-      <c r="B4" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="32" x14ac:dyDescent="0.4">
-      <c r="A5" s="3">
-        <v>63326</v>
-      </c>
-      <c r="B5" s="3">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="32" x14ac:dyDescent="0.4">
-      <c r="A6" s="3">
-        <v>3947</v>
-      </c>
-      <c r="B6" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="32" x14ac:dyDescent="0.4">
-      <c r="A7" s="3">
-        <v>1261</v>
-      </c>
-      <c r="B7" s="3">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="32" x14ac:dyDescent="0.4">
-      <c r="A8" s="3">
-        <v>1264</v>
-      </c>
-      <c r="B8" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
+    <row r="27" spans="1:2" ht="32" x14ac:dyDescent="0.4">
+      <c r="A27" s="1">
+        <v>1185</v>
+      </c>
+      <c r="B27" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="32" x14ac:dyDescent="0.4">
+      <c r="A28" s="1">
+        <v>1361</v>
+      </c>
+      <c r="B28" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="32" x14ac:dyDescent="0.4">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>